<commit_message>
Best so far for 1 and 7
</commit_message>
<xml_diff>
--- a/TestMNIST/MatlabCodes/final_4_9.xlsx
+++ b/TestMNIST/MatlabCodes/final_4_9.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E2"/>
@@ -409,38 +409,324 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
+        <v>0.33023845067334356</v>
+      </c>
+      <c r="B1">
         <v>0.33023845067334306</v>
       </c>
-      <c r="B1">
+      <c r="C1">
+        <v>0.33023845067334306</v>
+      </c>
+      <c r="D1">
         <v>0.33023845067334312</v>
       </c>
-      <c r="C1">
-        <v>0.33023845067334284</v>
-      </c>
-      <c r="D1">
-        <v>0.33023845067334279</v>
-      </c>
       <c r="E1">
+        <v>0.33023845067334395</v>
+      </c>
+      <c r="F1">
+        <v>0.33023845067334301</v>
+      </c>
+      <c r="G1">
+        <v>0.33023845067334306</v>
+      </c>
+      <c r="H1">
         <v>0.66976154932665688</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I1">
+        <v>0.70021443383503601</v>
+      </c>
+      <c r="J1">
+        <v>0.21214475203408711</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.66976154932665688</v>
+        <v>0.66976154932665755</v>
       </c>
       <c r="B2">
         <v>0.66976154932665688</v>
       </c>
       <c r="C2">
-        <v>0.66976154932665677</v>
+        <v>0.66976154932665688</v>
       </c>
       <c r="D2">
-        <v>0.66976154932665666</v>
+        <v>0.66976154932665688</v>
       </c>
       <c r="E2">
-        <v>0.33023845067334306</v>
+        <v>0.66976154932665777</v>
+      </c>
+      <c r="F2">
+        <v>0.66976154932665688</v>
+      </c>
+      <c r="G2">
+        <v>0.66976154932665688</v>
+      </c>
+      <c r="H2">
+        <v>0.33023845067334312</v>
+      </c>
+      <c r="I2">
+        <v>0.69535757471345483</v>
+      </c>
+      <c r="J2">
+        <v>0.51657409514763308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.41377429599751708</v>
+      </c>
+      <c r="B3">
+        <v>0.50436732656813088</v>
+      </c>
+      <c r="C3">
+        <v>0.23700111440535213</v>
+      </c>
+      <c r="D3">
+        <v>0.45424639982929521</v>
+      </c>
+      <c r="E3">
+        <v>0.72528016650558447</v>
+      </c>
+      <c r="F3">
+        <v>0.65427016926576187</v>
+      </c>
+      <c r="G3">
+        <v>0.41875930943216211</v>
+      </c>
+      <c r="H3">
+        <v>0.52195113596310561</v>
+      </c>
+      <c r="I3">
+        <v>0.5568379996040006</v>
+      </c>
+      <c r="J3">
+        <v>0.72812040591305638</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.45727218127258834</v>
+      </c>
+      <c r="B4">
+        <v>0.86368026343724835</v>
+      </c>
+      <c r="C4">
+        <v>0.65909783767747743</v>
+      </c>
+      <c r="D4">
+        <v>0.90776775696655065</v>
+      </c>
+      <c r="E4">
+        <v>0.72232268717178183</v>
+      </c>
+      <c r="F4">
+        <v>0.20900132975518945</v>
+      </c>
+      <c r="G4">
+        <v>0.87186895899712313</v>
+      </c>
+      <c r="H4">
+        <v>0.4809021818643579</v>
+      </c>
+      <c r="I4">
+        <v>0.18311104512541981</v>
+      </c>
+      <c r="J4">
+        <v>0.85753609750275017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.32708307875262382</v>
+      </c>
+      <c r="B5">
+        <v>0.48854385805588885</v>
+      </c>
+      <c r="C5">
+        <v>0.51470854573911218</v>
+      </c>
+      <c r="D5">
+        <v>0.2504780540911935</v>
+      </c>
+      <c r="E5">
+        <v>0.43128274379277143</v>
+      </c>
+      <c r="F5">
+        <v>0.4810841189188827</v>
+      </c>
+      <c r="G5">
+        <v>0.59932930849828503</v>
+      </c>
+      <c r="H5">
+        <v>0.36767133311574046</v>
+      </c>
+      <c r="I5">
+        <v>0.30775517309954503</v>
+      </c>
+      <c r="J5">
+        <v>0.42769863820655679</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.84457671979571269</v>
+      </c>
+      <c r="B6">
+        <v>0.34513057787093898</v>
+      </c>
+      <c r="C6">
+        <v>0.82650647044365755</v>
+      </c>
+      <c r="D6">
+        <v>0.57222733212599497</v>
+      </c>
+      <c r="E6">
+        <v>0.32232154646043459</v>
+      </c>
+      <c r="F6">
+        <v>0.36823890538403919</v>
+      </c>
+      <c r="G6">
+        <v>0.42029281733002266</v>
+      </c>
+      <c r="H6">
+        <v>0.19626191164983159</v>
+      </c>
+      <c r="I6">
+        <v>0.68000611845436265</v>
+      </c>
+      <c r="J6">
+        <v>0.55059082392537462</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.65672640444261432</v>
+      </c>
+      <c r="B7">
+        <v>0.83852081111067911</v>
+      </c>
+      <c r="C7">
+        <v>0.3718195205713008</v>
+      </c>
+      <c r="D7">
+        <v>0.6933961391417065</v>
+      </c>
+      <c r="E7">
+        <v>0.82415496818212741</v>
+      </c>
+      <c r="F7">
+        <v>0.57091844684780069</v>
+      </c>
+      <c r="G7">
+        <v>0.79075891545393695</v>
+      </c>
+      <c r="H7">
+        <v>0.63787964233791072</v>
+      </c>
+      <c r="I7">
+        <v>0.36096498031501684</v>
+      </c>
+      <c r="J7">
+        <v>0.69740022786375644</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.411966911950507</v>
+      </c>
+      <c r="B8">
+        <v>0.30834000459043148</v>
+      </c>
+      <c r="C8">
+        <v>0.68714409052882364</v>
+      </c>
+      <c r="D8">
+        <v>0.42751593828851037</v>
+      </c>
+      <c r="E8">
+        <v>0.12888216402819458</v>
+      </c>
+      <c r="F8">
+        <v>0.50275348294084454</v>
+      </c>
+      <c r="G8">
+        <v>0.16527677407517238</v>
+      </c>
+      <c r="H8">
+        <v>0.21835762379365584</v>
+      </c>
+      <c r="I8">
+        <v>0.62772746879403019</v>
+      </c>
+      <c r="J8">
+        <v>0.23206686003285043</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.8013817386997214</v>
+      </c>
+      <c r="B9">
+        <v>0.26813201522415536</v>
+      </c>
+      <c r="C9">
+        <v>0.49576293199215066</v>
+      </c>
+      <c r="D9">
+        <v>0.25708421868783415</v>
+      </c>
+      <c r="E9">
+        <v>0.40913716130695638</v>
+      </c>
+      <c r="F9">
+        <v>0.58593525001521629</v>
+      </c>
+      <c r="G9">
+        <v>0.43916598225066683</v>
+      </c>
+      <c r="H9">
+        <v>0.68417928246011595</v>
+      </c>
+      <c r="I9">
+        <v>0.18813455891470213</v>
+      </c>
+      <c r="J9">
+        <v>0.29161190370988271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.45005196975841349</v>
+      </c>
+      <c r="B10">
+        <v>0.54183266485166581</v>
+      </c>
+      <c r="C10">
+        <v>0.72606319232840166</v>
+      </c>
+      <c r="D10">
+        <v>0.32205730808574717</v>
+      </c>
+      <c r="E10">
+        <v>0.50191541617677493</v>
+      </c>
+      <c r="F10">
+        <v>0.89519478685417575</v>
+      </c>
+      <c r="G10">
+        <v>0.37195191630963387</v>
+      </c>
+      <c r="H10">
+        <v>0.73148886155516935</v>
+      </c>
+      <c r="I10">
+        <v>0.76154624719483155</v>
+      </c>
+      <c r="J10">
+        <v>0.45094056828122875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
z-score function with0 as second argument
</commit_message>
<xml_diff>
--- a/TestMNIST/MatlabCodes/final_4_9.xlsx
+++ b/TestMNIST/MatlabCodes/final_4_9.xlsx
@@ -411,19 +411,19 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.33023845067334356</v>
+        <v>8.4860496271119048E-4</v>
       </c>
       <c r="B1">
-        <v>0.33023845067334306</v>
+        <v>8.4860496271122962E-4</v>
       </c>
       <c r="C1">
-        <v>0.33023845067334306</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="D1">
-        <v>0.33023845067334312</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="E1">
-        <v>0.33023845067334395</v>
+        <v>8.4860496271118668E-4</v>
       </c>
       <c r="F1">
         <v>0.33023845067334301</v>
@@ -443,19 +443,19 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.66976154932665755</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="B2">
-        <v>0.66976154932665688</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="C2">
-        <v>0.66976154932665688</v>
+        <v>8.4860496271118668E-4</v>
       </c>
       <c r="D2">
-        <v>0.66976154932665688</v>
+        <v>8.4860496271118668E-4</v>
       </c>
       <c r="E2">
-        <v>0.66976154932665777</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="F2">
         <v>0.66976154932665688</v>

</xml_diff>

<commit_message>
best results for 1 and 9
</commit_message>
<xml_diff>
--- a/TestMNIST/MatlabCodes/final_4_9.xlsx
+++ b/TestMNIST/MatlabCodes/final_4_9.xlsx
@@ -414,16 +414,16 @@
         <v>8.4860496271119048E-4</v>
       </c>
       <c r="B1">
-        <v>8.4860496271122962E-4</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="C1">
-        <v>0.99915139503728889</v>
+        <v>8.4860496271118668E-4</v>
       </c>
       <c r="D1">
         <v>0.99915139503728889</v>
       </c>
       <c r="E1">
-        <v>8.4860496271118668E-4</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="F1">
         <v>0.33023845067334301</v>
@@ -446,16 +446,16 @@
         <v>0.99915139503728889</v>
       </c>
       <c r="B2">
+        <v>8.4860496271118733E-4</v>
+      </c>
+      <c r="C2">
         <v>0.99915139503728889</v>
       </c>
-      <c r="C2">
-        <v>8.4860496271118668E-4</v>
-      </c>
       <c r="D2">
-        <v>8.4860496271118668E-4</v>
+        <v>8.486049627111882E-4</v>
       </c>
       <c r="E2">
-        <v>0.99915139503728889</v>
+        <v>8.486049627111882E-4</v>
       </c>
       <c r="F2">
         <v>0.66976154932665688</v>
@@ -475,19 +475,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.41377429599751708</v>
+        <v>7.7231267282164154E-4</v>
       </c>
       <c r="B3">
-        <v>0.50436732656813088</v>
+        <v>0.99999998236568322</v>
       </c>
       <c r="C3">
-        <v>0.23700111440535213</v>
+        <v>7.7194901648280745E-2</v>
       </c>
       <c r="D3">
-        <v>0.45424639982929521</v>
+        <v>0.99998507526828129</v>
       </c>
       <c r="E3">
-        <v>0.72528016650558447</v>
+        <v>1.4766012930259687E-2</v>
       </c>
       <c r="F3">
         <v>0.65427016926576187</v>
@@ -507,19 +507,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.45727218127258834</v>
+        <v>1.9679869229992561E-3</v>
       </c>
       <c r="B4">
-        <v>0.86368026343724835</v>
+        <v>5.98665017412413E-2</v>
       </c>
       <c r="C4">
-        <v>0.65909783767747743</v>
+        <v>3.2102021747555274E-3</v>
       </c>
       <c r="D4">
-        <v>0.90776775696655065</v>
+        <v>1.7142080046726037E-3</v>
       </c>
       <c r="E4">
-        <v>0.72232268717178183</v>
+        <v>1.2204457330757168E-2</v>
       </c>
       <c r="F4">
         <v>0.20900132975518945</v>
@@ -539,19 +539,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.32708307875262382</v>
+        <v>1.9088910243797146E-4</v>
       </c>
       <c r="B5">
-        <v>0.48854385805588885</v>
+        <v>2.4889230184229396E-4</v>
       </c>
       <c r="C5">
-        <v>0.51470854573911218</v>
+        <v>3.699529291226178E-7</v>
       </c>
       <c r="D5">
-        <v>0.2504780540911935</v>
+        <v>2.7383873081581811E-7</v>
       </c>
       <c r="E5">
-        <v>0.43128274379277143</v>
+        <v>3.1800355378368657E-9</v>
       </c>
       <c r="F5">
         <v>0.4810841189188827</v>
@@ -571,19 +571,19 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.84457671979571269</v>
+        <v>0.99998869075193597</v>
       </c>
       <c r="B6">
-        <v>0.34513057787093898</v>
+        <v>0.98893180521330648</v>
       </c>
       <c r="C6">
-        <v>0.82650647044365755</v>
+        <v>2.6243185369630931E-7</v>
       </c>
       <c r="D6">
-        <v>0.57222733212599497</v>
+        <v>1.9229309587742243E-3</v>
       </c>
       <c r="E6">
-        <v>0.32232154646043459</v>
+        <v>0.99987500137649243</v>
       </c>
       <c r="F6">
         <v>0.36823890538403919</v>
@@ -603,19 +603,19 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.65672640444261432</v>
+        <v>1.2689150783167067E-3</v>
       </c>
       <c r="B7">
-        <v>0.83852081111067911</v>
+        <v>0.59381181692280627</v>
       </c>
       <c r="C7">
-        <v>0.3718195205713008</v>
+        <v>0.99796577853442459</v>
       </c>
       <c r="D7">
-        <v>0.6933961391417065</v>
+        <v>3.053333798289417E-2</v>
       </c>
       <c r="E7">
-        <v>0.82415496818212741</v>
+        <v>0.91146280733748342</v>
       </c>
       <c r="F7">
         <v>0.57091844684780069</v>
@@ -635,19 +635,19 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.411966911950507</v>
+        <v>0.99999999954399876</v>
       </c>
       <c r="B8">
-        <v>0.30834000459043148</v>
+        <v>4.436475871691599E-8</v>
       </c>
       <c r="C8">
-        <v>0.68714409052882364</v>
+        <v>0.96564921215380184</v>
       </c>
       <c r="D8">
-        <v>0.42751593828851037</v>
+        <v>8.0691226193160812E-2</v>
       </c>
       <c r="E8">
-        <v>0.12888216402819458</v>
+        <v>2.837932168242639E-5</v>
       </c>
       <c r="F8">
         <v>0.50275348294084454</v>
@@ -667,19 +667,19 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0.8013817386997214</v>
+        <v>0.91710009307730855</v>
       </c>
       <c r="B9">
-        <v>0.26813201522415536</v>
+        <v>0.99908427352419515</v>
       </c>
       <c r="C9">
-        <v>0.49576293199215066</v>
+        <v>0.278858128312238</v>
       </c>
       <c r="D9">
-        <v>0.25708421868783415</v>
+        <v>0.99999998996817252</v>
       </c>
       <c r="E9">
-        <v>0.40913716130695638</v>
+        <v>0.99999371477344556</v>
       </c>
       <c r="F9">
         <v>0.58593525001521629</v>
@@ -699,19 +699,19 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.45005196975841349</v>
+        <v>1.4441997333328998E-2</v>
       </c>
       <c r="B10">
-        <v>0.54183266485166581</v>
+        <v>0.99833913734828716</v>
       </c>
       <c r="C10">
-        <v>0.72606319232840166</v>
+        <v>0.97329473362624308</v>
       </c>
       <c r="D10">
-        <v>0.32205730808574717</v>
+        <v>0.99983680146317999</v>
       </c>
       <c r="E10">
-        <v>0.50191541617677493</v>
+        <v>0.99996867686606372</v>
       </c>
       <c r="F10">
         <v>0.89519478685417575</v>

</xml_diff>

<commit_message>
results code for 3 and 4 clustering
</commit_message>
<xml_diff>
--- a/TestMNIST/MatlabCodes/final_4_9.xlsx
+++ b/TestMNIST/MatlabCodes/final_4_9.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E2"/>
@@ -409,324 +409,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>8.4860496271119048E-4</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="B1">
+        <v>8.4860496271118733E-4</v>
+      </c>
+      <c r="C1">
         <v>0.99915139503728889</v>
       </c>
-      <c r="C1">
+      <c r="D1">
+        <v>8.4860496271107143E-4</v>
+      </c>
+      <c r="E1">
+        <v>0.99915139503728845</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8.4860496271125802E-4</v>
+      </c>
+      <c r="B2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="C2">
         <v>8.4860496271118668E-4</v>
       </c>
-      <c r="D1">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="E1">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="F1">
-        <v>0.33023845067334301</v>
-      </c>
-      <c r="G1">
-        <v>0.33023845067334306</v>
-      </c>
-      <c r="H1">
-        <v>0.66976154932665688</v>
-      </c>
-      <c r="I1">
-        <v>0.70021443383503601</v>
-      </c>
-      <c r="J1">
-        <v>0.21214475203408711</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="B2">
-        <v>8.4860496271118733E-4</v>
-      </c>
-      <c r="C2">
-        <v>0.99915139503728889</v>
-      </c>
       <c r="D2">
-        <v>8.486049627111882E-4</v>
+        <v>0.99915139503728867</v>
       </c>
       <c r="E2">
-        <v>8.486049627111882E-4</v>
-      </c>
-      <c r="F2">
-        <v>0.66976154932665688</v>
-      </c>
-      <c r="G2">
-        <v>0.66976154932665688</v>
-      </c>
-      <c r="H2">
-        <v>0.33023845067334312</v>
-      </c>
-      <c r="I2">
-        <v>0.69535757471345483</v>
-      </c>
-      <c r="J2">
-        <v>0.51657409514763308</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>7.7231267282164154E-4</v>
-      </c>
-      <c r="B3">
-        <v>0.99999998236568322</v>
-      </c>
-      <c r="C3">
-        <v>7.7194901648280745E-2</v>
-      </c>
-      <c r="D3">
-        <v>0.99998507526828129</v>
-      </c>
-      <c r="E3">
-        <v>1.4766012930259687E-2</v>
-      </c>
-      <c r="F3">
-        <v>0.65427016926576187</v>
-      </c>
-      <c r="G3">
-        <v>0.41875930943216211</v>
-      </c>
-      <c r="H3">
-        <v>0.52195113596310561</v>
-      </c>
-      <c r="I3">
-        <v>0.5568379996040006</v>
-      </c>
-      <c r="J3">
-        <v>0.72812040591305638</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1.9679869229992561E-3</v>
-      </c>
-      <c r="B4">
-        <v>5.98665017412413E-2</v>
-      </c>
-      <c r="C4">
-        <v>3.2102021747555274E-3</v>
-      </c>
-      <c r="D4">
-        <v>1.7142080046726037E-3</v>
-      </c>
-      <c r="E4">
-        <v>1.2204457330757168E-2</v>
-      </c>
-      <c r="F4">
-        <v>0.20900132975518945</v>
-      </c>
-      <c r="G4">
-        <v>0.87186895899712313</v>
-      </c>
-      <c r="H4">
-        <v>0.4809021818643579</v>
-      </c>
-      <c r="I4">
-        <v>0.18311104512541981</v>
-      </c>
-      <c r="J4">
-        <v>0.85753609750275017</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1.9088910243797146E-4</v>
-      </c>
-      <c r="B5">
-        <v>2.4889230184229396E-4</v>
-      </c>
-      <c r="C5">
-        <v>3.699529291226178E-7</v>
-      </c>
-      <c r="D5">
-        <v>2.7383873081581811E-7</v>
-      </c>
-      <c r="E5">
-        <v>3.1800355378368657E-9</v>
-      </c>
-      <c r="F5">
-        <v>0.4810841189188827</v>
-      </c>
-      <c r="G5">
-        <v>0.59932930849828503</v>
-      </c>
-      <c r="H5">
-        <v>0.36767133311574046</v>
-      </c>
-      <c r="I5">
-        <v>0.30775517309954503</v>
-      </c>
-      <c r="J5">
-        <v>0.42769863820655679</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0.99998869075193597</v>
-      </c>
-      <c r="B6">
-        <v>0.98893180521330648</v>
-      </c>
-      <c r="C6">
-        <v>2.6243185369630931E-7</v>
-      </c>
-      <c r="D6">
-        <v>1.9229309587742243E-3</v>
-      </c>
-      <c r="E6">
-        <v>0.99987500137649243</v>
-      </c>
-      <c r="F6">
-        <v>0.36823890538403919</v>
-      </c>
-      <c r="G6">
-        <v>0.42029281733002266</v>
-      </c>
-      <c r="H6">
-        <v>0.19626191164983159</v>
-      </c>
-      <c r="I6">
-        <v>0.68000611845436265</v>
-      </c>
-      <c r="J6">
-        <v>0.55059082392537462</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1.2689150783167067E-3</v>
-      </c>
-      <c r="B7">
-        <v>0.59381181692280627</v>
-      </c>
-      <c r="C7">
-        <v>0.99796577853442459</v>
-      </c>
-      <c r="D7">
-        <v>3.053333798289417E-2</v>
-      </c>
-      <c r="E7">
-        <v>0.91146280733748342</v>
-      </c>
-      <c r="F7">
-        <v>0.57091844684780069</v>
-      </c>
-      <c r="G7">
-        <v>0.79075891545393695</v>
-      </c>
-      <c r="H7">
-        <v>0.63787964233791072</v>
-      </c>
-      <c r="I7">
-        <v>0.36096498031501684</v>
-      </c>
-      <c r="J7">
-        <v>0.69740022786375644</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0.99999999954399876</v>
-      </c>
-      <c r="B8">
-        <v>4.436475871691599E-8</v>
-      </c>
-      <c r="C8">
-        <v>0.96564921215380184</v>
-      </c>
-      <c r="D8">
-        <v>8.0691226193160812E-2</v>
-      </c>
-      <c r="E8">
-        <v>2.837932168242639E-5</v>
-      </c>
-      <c r="F8">
-        <v>0.50275348294084454</v>
-      </c>
-      <c r="G8">
-        <v>0.16527677407517238</v>
-      </c>
-      <c r="H8">
-        <v>0.21835762379365584</v>
-      </c>
-      <c r="I8">
-        <v>0.62772746879403019</v>
-      </c>
-      <c r="J8">
-        <v>0.23206686003285043</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0.91710009307730855</v>
-      </c>
-      <c r="B9">
-        <v>0.99908427352419515</v>
-      </c>
-      <c r="C9">
-        <v>0.278858128312238</v>
-      </c>
-      <c r="D9">
-        <v>0.99999998996817252</v>
-      </c>
-      <c r="E9">
-        <v>0.99999371477344556</v>
-      </c>
-      <c r="F9">
-        <v>0.58593525001521629</v>
-      </c>
-      <c r="G9">
-        <v>0.43916598225066683</v>
-      </c>
-      <c r="H9">
-        <v>0.68417928246011595</v>
-      </c>
-      <c r="I9">
-        <v>0.18813455891470213</v>
-      </c>
-      <c r="J9">
-        <v>0.29161190370988271</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1.4441997333328998E-2</v>
-      </c>
-      <c r="B10">
-        <v>0.99833913734828716</v>
-      </c>
-      <c r="C10">
-        <v>0.97329473362624308</v>
-      </c>
-      <c r="D10">
-        <v>0.99983680146317999</v>
-      </c>
-      <c r="E10">
-        <v>0.99996867686606372</v>
-      </c>
-      <c r="F10">
-        <v>0.89519478685417575</v>
-      </c>
-      <c r="G10">
-        <v>0.37195191630963387</v>
-      </c>
-      <c r="H10">
-        <v>0.73148886155516935</v>
-      </c>
-      <c r="I10">
-        <v>0.76154624719483155</v>
-      </c>
-      <c r="J10">
-        <v>0.45094056828122875</v>
+        <v>8.4860496271078076E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
train model new with best so far for 1 and 0
</commit_message>
<xml_diff>
--- a/TestMNIST/MatlabCodes/final_4_9.xlsx
+++ b/TestMNIST/MatlabCodes/final_4_9.xlsx
@@ -401,46 +401,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0.99915139503728889</v>
       </c>
       <c r="B1">
-        <v>0.99915139503728889</v>
+        <v>8.4860496271118668E-4</v>
       </c>
       <c r="C1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="D1">
         <v>8.4860496271118733E-4</v>
       </c>
-      <c r="D1">
-        <v>0.99915139503728889</v>
-      </c>
       <c r="E1">
-        <v>0.99915139503728889</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.99915139503728867</v>
+      </c>
+      <c r="F1">
+        <v>8.4860496271118668E-4</v>
+      </c>
+      <c r="G1">
+        <v>8.4860496271118668E-4</v>
+      </c>
+      <c r="H1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="I1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="J1">
+        <v>8.4860496271126952E-4</v>
+      </c>
+      <c r="K1">
+        <v>8.4860496271121683E-4</v>
+      </c>
+      <c r="L1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="M1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="N1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="O1">
+        <v>8.4860496271114147E-4</v>
+      </c>
+      <c r="P1">
+        <v>8.4860496271121227E-4</v>
+      </c>
+      <c r="Q1">
+        <v>8.4860496271118733E-4</v>
+      </c>
+      <c r="R1">
+        <v>8.4860496271118668E-4</v>
+      </c>
+      <c r="S1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="T1">
+        <v>0.99915139503728889</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8.4860496271120761E-4</v>
+        <v>8.4860496271118668E-4</v>
       </c>
       <c r="B2">
-        <v>8.4860496271118668E-4</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="C2">
-        <v>0.99915139503728889</v>
+        <v>8.4860496271118733E-4</v>
       </c>
       <c r="D2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="E2">
+        <v>8.4860496271114668E-4</v>
+      </c>
+      <c r="F2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="G2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="H2">
         <v>8.4860496271118733E-4</v>
       </c>
-      <c r="E2">
-        <v>8.4860496271120989E-4</v>
+      <c r="I2">
+        <v>8.4860496271118733E-4</v>
+      </c>
+      <c r="J2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="K2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="L2">
+        <v>8.4860496271119417E-4</v>
+      </c>
+      <c r="M2">
+        <v>8.4860496271118668E-4</v>
+      </c>
+      <c r="N2">
+        <v>8.4860496271118668E-4</v>
+      </c>
+      <c r="O2">
+        <v>0.99915139503728867</v>
+      </c>
+      <c r="P2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="Q2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="R2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="S2">
+        <v>8.4860496271128817E-4</v>
+      </c>
+      <c r="T2">
+        <v>8.4860496271118668E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.94512698668994977</v>
+      </c>
+      <c r="B3">
+        <v>0.99953755535884092</v>
+      </c>
+      <c r="C3">
+        <v>2.6030005273385688E-2</v>
+      </c>
+      <c r="D3">
+        <v>1.3587496717803083E-4</v>
+      </c>
+      <c r="E3">
+        <v>4.7584009735105487E-2</v>
+      </c>
+      <c r="F3">
+        <v>2.3218843091358534E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Best yas_final code for 8 and 9 so far
</commit_message>
<xml_diff>
--- a/TestMNIST/MatlabCodes/final_4_9.xlsx
+++ b/TestMNIST/MatlabCodes/final_4_9.xlsx
@@ -411,34 +411,34 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="B1">
         <v>8.4860496271118668E-4</v>
       </c>
-      <c r="B1">
-        <v>8.4860496271118961E-4</v>
-      </c>
       <c r="C1">
-        <v>8.4860496271118354E-4</v>
+        <v>8.4860496271118668E-4</v>
       </c>
       <c r="D1">
-        <v>0.99915139503728889</v>
+        <v>8.4860496271118733E-4</v>
       </c>
       <c r="E1">
-        <v>0.99915139503728889</v>
+        <v>8.4860496271118733E-4</v>
       </c>
       <c r="F1">
-        <v>8.4860496271118213E-4</v>
+        <v>8.4860496271118506E-4</v>
       </c>
       <c r="G1">
+        <v>8.4860496271118441E-4</v>
+      </c>
+      <c r="H1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="I1">
         <v>8.4860496271118733E-4</v>
       </c>
-      <c r="H1">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="I1">
+      <c r="J1">
         <v>8.4860496271118668E-4</v>
-      </c>
-      <c r="J1">
-        <v>0.99915139503728889</v>
       </c>
       <c r="K1">
         <v>8.4860496271121683E-4</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.99915139503728889</v>
+        <v>8.4860496271118733E-4</v>
       </c>
       <c r="B2">
         <v>0.99915139503728889</v>
@@ -482,10 +482,10 @@
         <v>0.99915139503728889</v>
       </c>
       <c r="D2">
-        <v>8.4860496271118668E-4</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="E2">
-        <v>8.4860496271118354E-4</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="F2">
         <v>0.99915139503728889</v>
@@ -494,13 +494,13 @@
         <v>0.99915139503728889</v>
       </c>
       <c r="H2">
-        <v>8.4860496271118506E-4</v>
+        <v>8.4860496271118061E-4</v>
       </c>
       <c r="I2">
         <v>0.99915139503728889</v>
       </c>
       <c r="J2">
-        <v>8.4860496271118668E-4</v>
+        <v>0.99915139503728889</v>
       </c>
       <c r="K2">
         <v>0.99915139503728889</v>

</xml_diff>

<commit_message>
Best Code for 6 and 8 with Lateral
</commit_message>
<xml_diff>
--- a/TestMNIST/MatlabCodes/final_4_9.xlsx
+++ b/TestMNIST/MatlabCodes/final_4_9.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:J2"/>
@@ -409,218 +409,172 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.99915139503728889</v>
+        <v>8.4860496271118733E-4</v>
       </c>
       <c r="B1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="C1">
+        <v>8.4860496271119048E-4</v>
+      </c>
+      <c r="D1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="E1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="F1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="G1">
+        <v>8.4860496271118506E-4</v>
+      </c>
+      <c r="H1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="I1">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="J1">
+        <v>8.486049627111882E-4</v>
+      </c>
+      <c r="K1">
+        <v>0.97188478489631747</v>
+      </c>
+      <c r="L1">
+        <v>2.8639397975813746E-2</v>
+      </c>
+      <c r="M1">
+        <v>0.97292984900216473</v>
+      </c>
+      <c r="N1">
+        <v>0.97067021138044496</v>
+      </c>
+      <c r="O1">
+        <v>2.7329999473717219E-2</v>
+      </c>
+      <c r="P1">
+        <v>0.96825388299525472</v>
+      </c>
+      <c r="Q1">
+        <v>0.97154491528527054</v>
+      </c>
+      <c r="R1">
+        <v>2.7700904681008595E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="B2">
         <v>8.4860496271118668E-4</v>
       </c>
-      <c r="C1">
+      <c r="C2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="D2">
+        <v>8.4860496271118733E-4</v>
+      </c>
+      <c r="E2">
         <v>8.4860496271118668E-4</v>
       </c>
-      <c r="D1">
+      <c r="F2">
+        <v>8.4860496271118668E-4</v>
+      </c>
+      <c r="G2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="H2">
         <v>8.4860496271118733E-4</v>
       </c>
-      <c r="E1">
+      <c r="I2">
         <v>8.4860496271118733E-4</v>
       </c>
-      <c r="F1">
-        <v>8.4860496271118506E-4</v>
-      </c>
-      <c r="G1">
-        <v>8.4860496271118441E-4</v>
-      </c>
-      <c r="H1">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="I1">
-        <v>8.4860496271118733E-4</v>
-      </c>
-      <c r="J1">
-        <v>8.4860496271118668E-4</v>
-      </c>
-      <c r="K1">
-        <v>8.4860496271121683E-4</v>
-      </c>
-      <c r="L1">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="M1">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="N1">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="O1">
-        <v>8.4860496271114147E-4</v>
-      </c>
-      <c r="P1">
-        <v>8.4860496271121227E-4</v>
-      </c>
-      <c r="Q1">
-        <v>8.4860496271118733E-4</v>
-      </c>
-      <c r="R1">
-        <v>8.4860496271118668E-4</v>
-      </c>
-      <c r="S1">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="T1">
-        <v>0.99915139503728889</v>
+      <c r="J2">
+        <v>0.99915139503728889</v>
+      </c>
+      <c r="K2">
+        <v>1.2508144314743703E-5</v>
+      </c>
+      <c r="L2">
+        <v>0.99998743903815623</v>
+      </c>
+      <c r="M2">
+        <v>1.2401836684912634E-5</v>
+      </c>
+      <c r="N2">
+        <v>1.2630028443166567E-5</v>
+      </c>
+      <c r="O2">
+        <v>0.99998757160326435</v>
+      </c>
+      <c r="P2">
+        <v>1.2867508786415157E-5</v>
+      </c>
+      <c r="Q2">
+        <v>1.2542427807117759E-5</v>
+      </c>
+      <c r="R2">
+        <v>0.99998753383854921</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>8.4860496271118733E-4</v>
-      </c>
-      <c r="B2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="C2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="D2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="E2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="F2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="G2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="H2">
-        <v>8.4860496271118061E-4</v>
-      </c>
-      <c r="I2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="J2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="K2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="L2">
-        <v>8.4860496271119417E-4</v>
-      </c>
-      <c r="M2">
-        <v>8.4860496271118668E-4</v>
-      </c>
-      <c r="N2">
-        <v>8.4860496271118668E-4</v>
-      </c>
-      <c r="O2">
-        <v>0.99915139503728867</v>
-      </c>
-      <c r="P2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="Q2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="R2">
-        <v>0.99915139503728889</v>
-      </c>
-      <c r="S2">
-        <v>8.4860496271128817E-4</v>
-      </c>
-      <c r="T2">
-        <v>8.4860496271118668E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.94512698668994977</v>
+        <v>4.8063889852499467E-4</v>
       </c>
       <c r="B3">
-        <v>0.99953755535884092</v>
+        <v>4.245959336349017E-4</v>
       </c>
       <c r="C3">
-        <v>2.6030005273385688E-2</v>
+        <v>0.99957028480179866</v>
       </c>
       <c r="D3">
-        <v>1.3587496717803083E-4</v>
+        <v>0.99973486265693867</v>
       </c>
       <c r="E3">
-        <v>4.7584009735105487E-2</v>
+        <v>6.2563452774726811E-4</v>
       </c>
       <c r="F3">
-        <v>2.3218843091358534E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>5</v>
+        <v>0.99959082355548412</v>
+      </c>
+      <c r="G3">
+        <v>0.99966295245495473</v>
+      </c>
+      <c r="H3">
+        <v>0.99956946616933584</v>
+      </c>
+      <c r="I3">
+        <v>5.0085826626883453E-4</v>
+      </c>
+      <c r="J3">
+        <v>0.99958257866751143</v>
+      </c>
+      <c r="K3">
+        <v>0.9995678008126766</v>
+      </c>
+      <c r="L3">
+        <v>4.2585325061390974E-4</v>
+      </c>
+      <c r="M3">
+        <v>0.99955445794488706</v>
+      </c>
+      <c r="N3">
+        <v>0.9995821782083385</v>
+      </c>
+      <c r="O3">
+        <v>4.4213443936560006E-4</v>
+      </c>
+      <c r="P3">
+        <v>0.99960769098731972</v>
+      </c>
+      <c r="Q3">
+        <v>0.99957194052579035</v>
+      </c>
+      <c r="R3">
+        <v>4.3737514435670161E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>